<commit_message>
code, structure and data updates
Includes all input data (except assessments)
</commit_message>
<xml_diff>
--- a/input/tables_extraction/CMS/CMS.xlsx
+++ b/input/tables_extraction/CMS/CMS.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>indic_id</t>
   </si>
   <si>
-    <t>indicators</t>
+    <t>indicator</t>
+  </si>
+  <si>
+    <t>indicators_matched</t>
   </si>
   <si>
     <t>SPMS_1_1</t>
@@ -65,16 +68,25 @@
     <t>SPMS_8_1_1_8</t>
   </si>
   <si>
+    <t>red list index of species survival for cms-listed bird species</t>
+  </si>
+  <si>
     <t>Red List Index (CMS-listed bird species)</t>
   </si>
   <si>
     <t>SPMS_8_1_2_9</t>
   </si>
   <si>
+    <t>red list index of species survival for migratory bird species</t>
+  </si>
+  <si>
     <t>Red List Index (migratory bird species)</t>
   </si>
   <si>
     <t>SPMS_8_1_3_10</t>
+  </si>
+  <si>
+    <t>red list index of species survival for cms-listed bird and mammal species</t>
   </si>
   <si>
     <t>Red List Index (CMS-listed bird and mammal species)</t>
@@ -453,6 +465,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="25.63"/>
+    <col customWidth="1" min="2" max="2" width="36.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -462,71 +475,97 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -553,12 +592,14 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -585,12 +626,14 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -617,52 +660,69 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -689,12 +749,14 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -721,66 +783,90 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -800,17 +886,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">

</xml_diff>